<commit_message>
Updates monthly task log and Excel file.
Updates the monthly task log with November's activities.
This includes analysis, modifications, and check-in tasks related to
various financial and administrative processes.

Also updates a related Excel file, likely containing data or configurations
relevant to the tasks logged in the markdown file.
</commit_message>
<xml_diff>
--- a/춘천시20251031미이체분불일치원인분석20251125.xlsx
+++ b/춘천시20251031미이체분불일치원인분석20251125.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\sidogeumgo_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD55012B-6FCD-4001-BD3A-B8FC2333DEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7B811C-6AEB-48C3-9679-CA5EC80BF940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1397,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y43" workbookViewId="0">
-      <selection activeCell="Y47" sqref="Y47:Z239"/>
+    <sheetView tabSelected="1" topLeftCell="Y41" workbookViewId="0">
+      <selection activeCell="Z53" sqref="Z53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2785,7 +2785,7 @@
       <c r="AE53" s="8">
         <v>527787210</v>
       </c>
-      <c r="AG53" s="9" t="b">
+      <c r="AG53" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -10126,7 +10126,7 @@
       <c r="AE233" s="8">
         <v>426408784</v>
       </c>
-      <c r="AG233" s="9" t="b">
+      <c r="AG233" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>

</xml_diff>